<commit_message>
Corrections du dossier + shell pytalismane
</commit_message>
<xml_diff>
--- a/dossiers/Final - Suivi des corrections.xlsx
+++ b/dossiers/Final - Suivi des corrections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\dossiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1639D4CF-3EC9-4D03-A398-B813AB2B51F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145E1147-AA59-4566-B657-9CF7E77AF177}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -643,6 +643,9 @@
       <c r="C21" s="3">
         <v>61</v>
       </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C22" s="3">
@@ -675,6 +678,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
       <c r="C25" s="3">
         <v>65</v>
       </c>
@@ -808,11 +814,11 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D41">
         <f>SUM(A4:A40)+SUM(D4:D37)</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E41" s="5">
         <f>D41/77</f>
-        <v>0.58441558441558439</v>
+        <v>0.61038961038961037</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Corrections du dossier et recalculs
</commit_message>
<xml_diff>
--- a/dossiers/Final - Suivi des corrections.xlsx
+++ b/dossiers/Final - Suivi des corrections.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\dossiers\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145E1147-AA59-4566-B657-9CF7E77AF177}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Corrigé (cpt)</t>
   </si>
@@ -39,11 +33,17 @@
   <si>
     <t>outil de =&gt; étendre à une classe sémantique</t>
   </si>
+  <si>
+    <t>Reste (cpt)</t>
+  </si>
+  <si>
+    <t>Reste (%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,7 +112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -123,6 +123,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,26 +218,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,23 +253,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -461,11 +428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -689,6 +656,9 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>1</v>
+      </c>
       <c r="C26" s="3">
         <v>66</v>
       </c>
@@ -713,6 +683,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
       <c r="C29" s="3">
         <v>69</v>
       </c>
@@ -729,6 +702,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
       <c r="C31" s="3">
         <v>71</v>
       </c>
@@ -744,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>1</v>
       </c>
@@ -755,7 +731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C34" s="3">
         <v>74</v>
       </c>
@@ -763,7 +739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>1</v>
       </c>
@@ -774,7 +750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>1</v>
       </c>
@@ -785,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>1</v>
       </c>
@@ -796,37 +772,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D41">
         <f>SUM(A4:A40)+SUM(D4:D37)</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E41" s="5">
         <f>D41/77</f>
-        <v>0.61038961038961037</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.64935064935064934</v>
+      </c>
+      <c r="F41">
+        <f>77-D41</f>
+        <v>27</v>
+      </c>
+      <c r="G41" s="6">
+        <f>1-E41</f>
+        <v>0.35064935064935066</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
         <v>0</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -836,7 +826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -848,7 +838,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>